<commit_message>
add code for update source from github
</commit_message>
<xml_diff>
--- a/github.xlsx
+++ b/github.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Dk kí 1 tài khoản</t>
   </si>
@@ -321,13 +321,28 @@
   </si>
   <si>
     <t>add tat ca trong foder</t>
+  </si>
+  <si>
+    <t>git fetch mleung</t>
+  </si>
+  <si>
+    <t>This will create a new remote branch called 'mleung/master'. Now we are ready to merge the code from the remote repository.</t>
+  </si>
+  <si>
+    <t>git merge mleung/master</t>
+  </si>
+  <si>
+    <t>Now we can fetch all the changes from mleung's code base.</t>
+  </si>
+  <si>
+    <t>update source code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,8 +404,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +421,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -468,6 +495,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -813,14 +845,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1048,7 +1081,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="1:8">
       <c r="B50" t="s">
         <v>49</v>
       </c>
@@ -1056,17 +1089,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="1:8">
       <c r="D51" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="1:8">
       <c r="D52" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="1:8">
       <c r="B55" t="s">
         <v>52</v>
       </c>
@@ -1077,10 +1110,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="1:8">
       <c r="D56" s="9"/>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="1:8">
       <c r="B58" t="s">
         <v>55</v>
       </c>
@@ -1090,6 +1123,44 @@
       <c r="E58" t="s">
         <v>54</v>
       </c>
+    </row>
+    <row r="61" spans="1:8" ht="19.5">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="1:8" ht="45.75">
+      <c r="B63" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>